<commit_message>
Give citation for euro data
</commit_message>
<xml_diff>
--- a/data/euro.xlsx
+++ b/data/euro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\Temp data folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3C1644-270A-4F5F-B270-6AE10C295AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB097FF-6903-4079-A4F7-7B06F70D4654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-8250" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>case</t>
   </si>
@@ -42,6 +42,42 @@
   </si>
   <si>
     <t>batch</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>The Weight of Euro Coins: Its Distribution Might Not Be As Normal As You Would Expect</t>
+  </si>
+  <si>
+    <t>Ziv Shkedy, Marc Aerts, and Herman Callaert</t>
+  </si>
+  <si>
+    <t>Hasselt University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal of Statistics Education Volume 14, Number 2 (2006), </t>
+  </si>
+  <si>
+    <t>jse.amstat.org/v14n2/datasets.aerts.html</t>
+  </si>
+  <si>
+    <t>The National Bank of Belgium claims that the 1 Euro coin weighs 7.5 grams.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Belgian bank allowed students at Hasselt University to "borrow" 2000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">newly-minted one-Euro coins. </t>
+  </si>
+  <si>
+    <t>Each coin was weighed individually, and the masses were recorded in grams.</t>
+  </si>
+  <si>
+    <t>Incidentally, the coins were bundled in eight batches of 250 coins each.</t>
+  </si>
+  <si>
+    <t>reference</t>
   </si>
 </sst>
 </file>
@@ -417,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2001"/>
+  <dimension ref="A1:D2001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,8 +471,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -446,8 +485,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -457,8 +499,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -468,8 +513,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -479,8 +527,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -490,8 +541,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -502,7 +556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -512,8 +566,11 @@
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -523,8 +580,11 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -534,8 +594,11 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -545,8 +608,11 @@
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -556,8 +622,11 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -567,8 +636,11 @@
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -579,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -590,7 +662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -22438,6 +22510,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>